<commit_message>
JavaDoc generiert und Protokoll erweitert
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung.xlsx
+++ b/Zeitaufzeichnung.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Dauer in Std.</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>Design Neuüberlegungen</t>
+  </si>
+  <si>
+    <t>Design Vorlage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desgin Umsetzung und RM </t>
+  </si>
+  <si>
+    <t>Fehler überarbeitung FK</t>
+  </si>
+  <si>
+    <t>Stedronsky</t>
   </si>
 </sst>
 </file>
@@ -159,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -172,6 +184,8 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -455,7 +469,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -489,7 +503,7 @@
       </c>
       <c r="D2" s="6">
         <f>SUM(A:A)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -502,7 +516,9 @@
       <c r="C3" s="11">
         <v>42024</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
@@ -516,19 +532,37 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12">
+        <v>42042</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="5"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="13">
+        <v>42044</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="9">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="12">
+        <v>42045</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>

</xml_diff>